<commit_message>
Teste de busca pela lupa falha e sucesso concluido com sucesso com report e print
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoAppiumTDD\src\test\java\br\com\rsinet\HUB_Appium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DDA220E-C4C6-4425-B738-643828DB6D73}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA93A07-D90B-4AE6-B76D-30AAF1690DB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -141,7 +141,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -160,6 +160,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF3300"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -173,7 +185,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -187,18 +199,25 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF3300"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -509,7 +528,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
   <dimension ref="A1:H6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -645,22 +664,22 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:H11"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.88671875" style="2"/>
     <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="8.88671875" style="2"/>
-    <col min="5" max="5" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="3" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>8</v>
       </c>
@@ -670,67 +689,95 @@
       <c r="C1" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="D1" s="3" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="E2" s="8">
+      <c r="D2" s="7">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="7" t="s">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="8" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="7" t="s">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="9" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B6" s="2" t="s">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="8"/>
+      <c r="B5" s="9"/>
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="8"/>
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="10"/>
+      <c r="B10" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C10" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="B7" s="2" t="s">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="10"/>
+      <c r="B11" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C11" s="10" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="F8" s="5"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H11" s="6"/>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="10"/>
+      <c r="B12" s="10"/>
+      <c r="C12" s="10"/>
+      <c r="E12" s="5"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="10"/>
+      <c r="B13" s="10"/>
+      <c r="C13" s="10"/>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="10"/>
+      <c r="B14" s="10"/>
+      <c r="C14" s="10"/>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="G15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Teste busca clique sucesso e falha concluido com report e print
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoAppiumTDD\src\test\java\br\com\rsinet\HUB_Appium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFA93A07-D90B-4AE6-B76D-30AAF1690DB9}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF97C55-3649-4F4E-879A-460B5D6F4CFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
   </bookViews>
   <sheets>
     <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
@@ -32,10 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="26">
-  <si>
-    <t>LastName</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -49,9 +46,6 @@
     <t>Cordeiro</t>
   </si>
   <si>
-    <t>City</t>
-  </si>
-  <si>
     <t>Osasco</t>
   </si>
   <si>
@@ -64,18 +58,12 @@
     <t>nomeProduto</t>
   </si>
   <si>
-    <t>Speakers</t>
-  </si>
-  <si>
     <t>HP USB 3 Button Optical Mouse</t>
   </si>
   <si>
     <t>Bose Soundlink Bluetooth Speaker III</t>
   </si>
   <si>
-    <t>Mice</t>
-  </si>
-  <si>
     <t>Descricao</t>
   </si>
   <si>
@@ -85,9 +73,6 @@
     <t>Falha</t>
   </si>
   <si>
-    <t>Laptops</t>
-  </si>
-  <si>
     <t>HP Chromebook 14 G1(ENERGY STAR)</t>
   </si>
   <si>
@@ -97,19 +82,52 @@
     <t>Mochila</t>
   </si>
   <si>
-    <t>FirstName</t>
-  </si>
-  <si>
-    <t>UserPass</t>
-  </si>
-  <si>
     <t>Email</t>
   </si>
   <si>
-    <t>PhoneNumber</t>
-  </si>
-  <si>
     <t>Quantidade</t>
+  </si>
+  <si>
+    <t>LAPTOPS</t>
+  </si>
+  <si>
+    <t>MICE</t>
+  </si>
+  <si>
+    <t>SPEAKERS</t>
+  </si>
+  <si>
+    <t>TABLETS</t>
+  </si>
+  <si>
+    <t>HEADPHONES</t>
+  </si>
+  <si>
+    <t>Beats Studio 2 Over-Ear Matte</t>
+  </si>
+  <si>
+    <t>HP Elitepad 1000 G2 Tablet</t>
+  </si>
+  <si>
+    <t>Usuario</t>
+  </si>
+  <si>
+    <t>Senha</t>
+  </si>
+  <si>
+    <t>Primeiro Nome</t>
+  </si>
+  <si>
+    <t>Ultimo Nome</t>
+  </si>
+  <si>
+    <t>Numero</t>
+  </si>
+  <si>
+    <t>Cidade</t>
+  </si>
+  <si>
+    <t>18lPxy</t>
   </si>
 </sst>
 </file>
@@ -141,7 +159,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -172,6 +190,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -199,14 +223,14 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -526,258 +550,238 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:I6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="12.21875" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H1" s="1"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="F1" s="3" t="s">
+      <c r="C2" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F2" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D4" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C5" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="H6" s="5"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="4"/>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="I6" s="5"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="A2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
-    <hyperlink ref="B2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
-    <hyperlink ref="A3" r:id="rId3" xr:uid="{E6C3CACA-3A5A-4CAD-82C5-D039F92D733C}"/>
-    <hyperlink ref="B3" r:id="rId4" xr:uid="{DD4376EB-C6F7-4AFF-966F-A20928D92B9D}"/>
-    <hyperlink ref="A4" r:id="rId5" xr:uid="{448D612A-5394-4591-AAB7-E6BC8C7667B1}"/>
-    <hyperlink ref="B4" r:id="rId6" xr:uid="{2DE44A87-009E-4ADB-B135-BA659499AA57}"/>
-    <hyperlink ref="A5" r:id="rId7" xr:uid="{4F212B3A-907F-4CD1-B5C1-DC1067447132}"/>
-    <hyperlink ref="B5" r:id="rId8" xr:uid="{79A6EDF3-1D65-40AB-A76F-25B083FE565B}"/>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
   </hyperlinks>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId9"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:G15"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L7" sqref="L7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
+    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="8.88671875" style="2"/>
-    <col min="4" max="4" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="3" max="6" width="8.88671875" style="2"/>
+    <col min="7" max="7" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="3" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="C2" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="G2" s="10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C6" s="8" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="8" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="9" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="9"/>
+      <c r="B10" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="9" t="s">
+      <c r="C10" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="9" t="s">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="B11" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="D2" s="7">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B3" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A4" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A5" s="8"/>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A6" s="8"/>
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:7" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A10" s="10"/>
-      <c r="B10" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A11" s="10"/>
-      <c r="B11" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="10" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A12" s="10"/>
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="E12" s="5"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A13" s="10"/>
-      <c r="B13" s="10"/>
-      <c r="C13" s="10"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A14" s="10"/>
-      <c r="B14" s="10"/>
-      <c r="C14" s="10"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="G15" s="6"/>
+      <c r="C11" s="9" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="H12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="B13" s="9"/>
+      <c r="C13" s="9"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="J15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>

</xml_diff>

<commit_message>
Ajustes no report dos testes
</commit_message>
<xml_diff>
--- a/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
+++ b/src/test/java/br/com/rsinet/HUB_Appium/TestData/BancoDados.xlsx
@@ -1,24 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abdiel.cordeiro\Documents\Projetos\eclipse-workspace\projetoAppiumTDD\src\test\java\br\com\rsinet\HUB_Appium\TestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AAF97C55-3649-4F4E-879A-460B5D6F4CFC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{AAF97C55-3649-4F4E-879A-460B5D6F4CFC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}"/>
+    <workbookView windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{C4F5F6C9-57A0-43D3-9FA4-F5EF18E402B6}" yWindow="-108"/>
   </bookViews>
   <sheets>
-    <sheet name="Cadastro" sheetId="1" r:id="rId1"/>
-    <sheet name="Pesquisa" sheetId="2" r:id="rId2"/>
+    <sheet name="Cadastro" r:id="rId1" sheetId="1"/>
+    <sheet name="Pesquisa" r:id="rId2" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="33">
   <si>
     <t>Trocar@123</t>
   </si>
@@ -128,12 +128,16 @@
   </si>
   <si>
     <t>18lPxy</t>
+  </si>
+  <si>
+    <t>sI5pfp</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -207,36 +211,36 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="11">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="3" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="0" numFmtId="49" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf applyFill="1" borderId="0" fillId="4" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="5" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyNumberFormat="1" borderId="0" fillId="6" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FFFF3300"/>
@@ -258,10 +262,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -296,7 +300,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin panose="020F0302020204030204" typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -348,7 +352,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin panose="020F0502020204030204" typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -459,21 +463,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -490,7 +494,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -542,15 +546,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5D6D5505-1405-49EC-A52B-B536267B1E1D}">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="K11" sqref="K11"/>
@@ -558,13 +562,13 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="2"/>
-    <col min="2" max="2" width="11.109375" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" style="2" customWidth="1"/>
-    <col min="5" max="5" width="12.21875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.44140625" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" style="2" width="8.88671875" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="11.109375" collapsed="false"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="26.44140625" collapsed="false"/>
+    <col min="4" max="4" customWidth="true" style="2" width="13.6640625" collapsed="false"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="12.21875" collapsed="false"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="13.44140625" collapsed="false"/>
+    <col min="7" max="16384" style="2" width="8.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.3">
@@ -593,7 +597,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
@@ -643,17 +647,17 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
-    <hyperlink ref="C2" r:id="rId2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
+    <hyperlink r:id="rId1" ref="B2" xr:uid="{46AC47A1-1F89-45AF-8C7B-F4A195208066}"/>
+    <hyperlink r:id="rId2" ref="C2" xr:uid="{85BD8E5A-7C04-41EF-BADE-536F55EA589D}"/>
   </hyperlinks>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId3"/>
+  <pageMargins bottom="0.78740157499999996" footer="0.31496062000000002" header="0.31496062000000002" left="0.511811024" right="0.511811024" top="0.78740157499999996"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId3" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
-  <dimension ref="A1:J15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EB9334BD-5787-4860-8F04-DE32560FFDB3}">
+  <dimension ref="A1:K15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L7" sqref="L7"/>
@@ -661,11 +665,11 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="6" width="8.88671875" style="2"/>
-    <col min="7" max="7" width="10.88671875" style="2" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="8.88671875" style="2"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="12.33203125" collapsed="false"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="36.6640625" collapsed="false"/>
+    <col min="3" max="6" style="2" width="8.88671875" collapsed="false"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="10.88671875" collapsed="false"/>
+    <col min="8" max="16384" style="2" width="8.88671875" collapsed="false"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.3">
@@ -743,9 +747,9 @@
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="8" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="9" spans="1:10" ht="13.8" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row customHeight="1" ht="13.8" r="7" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row customHeight="1" ht="13.8" r="8" spans="1:10" x14ac:dyDescent="0.3"/>
+    <row customHeight="1" ht="13.8" r="9" spans="1:10" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" s="9"/>
       <c r="B10" s="9" t="s">
@@ -784,7 +788,7 @@
       <c r="J15" s="6"/>
     </row>
   </sheetData>
-  <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageMargins bottom="0.78740157499999996" footer="0.31496062000000002" header="0.31496062000000002" left="0.511811024" right="0.511811024" top="0.78740157499999996"/>
+  <pageSetup horizontalDpi="300" orientation="portrait" paperSize="9" r:id="rId1" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>